<commit_message>
Add dropdown to tiny_example.md and readme.md.
</commit_message>
<xml_diff>
--- a/tiny_example.xlsx
+++ b/tiny_example.xlsx
@@ -15,10 +15,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t xml:space="preserve">Accrual Fractions
 </t>
+  </si>
+  <si>
+    <t>convention</t>
+  </si>
+  <si>
+    <t>ACT365</t>
   </si>
   <si>
     <t>valueDate</t>
@@ -92,10 +98,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -395,7 +402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -412,28 +419,41 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="n">
-        <v>43308</v>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>43308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="n">
         <v>43400</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4">
-        <f>QSA.GetYearFraction(C3,C4,"ACT365")</f>
+    <row r="7" spans="1:3">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <f>QSA.GetYearFraction(C4,C5,C3)</f>
         <v/>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="C3" type="list">
+      <formula1>"ACT365,ACT360,_30360"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>